<commit_message>
v1.6 edited about page, edited site colors
</commit_message>
<xml_diff>
--- a/Categories.xlsx
+++ b/Categories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Al\Documents\ByteSizeArxiv\Abstracts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neerajsudhakar/BSA_Web_MVP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A434C2A1-339B-4AF5-8F7F-2665D0DB7571}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C274C9-206A-004A-8F20-B1B9B468F83B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1FDBD104-F759-4528-9157-7D799DE775EC}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{1FDBD104-F759-4528-9157-7D799DE775EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -497,9 +497,6 @@
     <t xml:space="preserve">nlin.PS </t>
   </si>
   <si>
-    <t>Pattern Formation and Solitons</t>
-  </si>
-  <si>
     <t xml:space="preserve">cs.AI </t>
   </si>
   <si>
@@ -912,6 +909,9 @@
   </si>
   <si>
     <t>Theoretical Economics</t>
+  </si>
+  <si>
+    <t>Pattern Formation and Solutons</t>
   </si>
 </sst>
 </file>
@@ -1295,15 +1295,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D48CA84-7451-4B0B-8098-0AC9374BDE6F}">
   <dimension ref="A1:B158"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="81.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="81.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1311,7 +1313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1319,7 +1321,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1327,7 +1329,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1335,7 +1337,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1343,7 +1345,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1351,7 +1353,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1359,7 +1361,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1367,7 +1369,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -1375,7 +1377,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -1383,7 +1385,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -1391,7 +1393,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -1399,7 +1401,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -1407,7 +1409,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -1415,7 +1417,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
@@ -1423,7 +1425,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
@@ -1431,7 +1433,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
@@ -1439,7 +1441,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -1447,7 +1449,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>33</v>
       </c>
@@ -1455,7 +1457,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>35</v>
       </c>
@@ -1463,7 +1465,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>37</v>
       </c>
@@ -1471,7 +1473,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>39</v>
       </c>
@@ -1479,7 +1481,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
@@ -1487,7 +1489,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>43</v>
       </c>
@@ -1495,7 +1497,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>45</v>
       </c>
@@ -1503,7 +1505,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>47</v>
       </c>
@@ -1511,7 +1513,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>49</v>
       </c>
@@ -1519,7 +1521,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>51</v>
       </c>
@@ -1527,7 +1529,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>53</v>
       </c>
@@ -1535,7 +1537,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>55</v>
       </c>
@@ -1543,7 +1545,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>57</v>
       </c>
@@ -1551,7 +1553,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>59</v>
       </c>
@@ -1559,7 +1561,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>61</v>
       </c>
@@ -1567,7 +1569,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>63</v>
       </c>
@@ -1575,7 +1577,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>65</v>
       </c>
@@ -1583,7 +1585,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>67</v>
       </c>
@@ -1591,7 +1593,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>69</v>
       </c>
@@ -1599,7 +1601,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>71</v>
       </c>
@@ -1607,7 +1609,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>73</v>
       </c>
@@ -1615,7 +1617,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>75</v>
       </c>
@@ -1623,7 +1625,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>14</v>
       </c>
@@ -1631,7 +1633,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>77</v>
       </c>
@@ -1639,7 +1641,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>79</v>
       </c>
@@ -1647,7 +1649,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>81</v>
       </c>
@@ -1655,7 +1657,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>83</v>
       </c>
@@ -1663,7 +1665,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>85</v>
       </c>
@@ -1671,7 +1673,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>87</v>
       </c>
@@ -1679,7 +1681,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>89</v>
       </c>
@@ -1687,7 +1689,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>91</v>
       </c>
@@ -1695,7 +1697,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>93</v>
       </c>
@@ -1703,7 +1705,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>95</v>
       </c>
@@ -1711,7 +1713,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>97</v>
       </c>
@@ -1719,7 +1721,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>99</v>
       </c>
@@ -1727,7 +1729,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>101</v>
       </c>
@@ -1735,7 +1737,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>103</v>
       </c>
@@ -1743,7 +1745,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>105</v>
       </c>
@@ -1751,7 +1753,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>107</v>
       </c>
@@ -1759,7 +1761,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>109</v>
       </c>
@@ -1767,7 +1769,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>111</v>
       </c>
@@ -1775,7 +1777,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>113</v>
       </c>
@@ -1783,7 +1785,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>115</v>
       </c>
@@ -1791,7 +1793,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>117</v>
       </c>
@@ -1799,7 +1801,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>119</v>
       </c>
@@ -1807,7 +1809,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>121</v>
       </c>
@@ -1815,7 +1817,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>123</v>
       </c>
@@ -1823,7 +1825,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>125</v>
       </c>
@@ -1831,7 +1833,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>127</v>
       </c>
@@ -1839,7 +1841,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>129</v>
       </c>
@@ -1847,7 +1849,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>131</v>
       </c>
@@ -1855,7 +1857,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>133</v>
       </c>
@@ -1863,7 +1865,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>135</v>
       </c>
@@ -1871,7 +1873,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>137</v>
       </c>
@@ -1879,7 +1881,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>139</v>
       </c>
@@ -1887,7 +1889,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>14</v>
       </c>
@@ -1895,7 +1897,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>14</v>
       </c>
@@ -1903,7 +1905,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>141</v>
       </c>
@@ -1911,7 +1913,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>143</v>
       </c>
@@ -1919,7 +1921,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>145</v>
       </c>
@@ -1927,7 +1929,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>147</v>
       </c>
@@ -1935,15 +1937,15 @@
         <v>148</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>149</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>14</v>
       </c>
@@ -1951,327 +1953,327 @@
         <v>14</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B82" s="1" t="s">
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+      <c r="B83" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B83" s="1" t="s">
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+      <c r="B84" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B84" s="1" t="s">
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+      <c r="B85" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B85" s="1" t="s">
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+      <c r="B86" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B86" s="1" t="s">
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+      <c r="B87" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B87" s="1" t="s">
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+      <c r="B88" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B88" s="1" t="s">
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+      <c r="B89" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B89" s="1" t="s">
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
+      <c r="B90" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B90" s="1" t="s">
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
+      <c r="B91" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B91" s="1" t="s">
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
+      <c r="B92" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B92" s="1" t="s">
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
+      <c r="B93" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B93" s="1" t="s">
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
+      <c r="B94" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B94" s="1" t="s">
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
+      <c r="B95" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B95" s="1" t="s">
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
+      <c r="B96" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B96" s="1" t="s">
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
+      <c r="B97" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B97" s="1" t="s">
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
+      <c r="B98" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B98" s="1" t="s">
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
+      <c r="B99" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B99" s="1" t="s">
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="1" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
+      <c r="B100" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B100" s="1" t="s">
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
+      <c r="B101" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B101" s="1" t="s">
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
+      <c r="B102" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B102" s="1" t="s">
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
         <v>192</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
-        <v>193</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B104" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B104" s="1" t="s">
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" s="1" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
+      <c r="B105" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B105" s="1" t="s">
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="1" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
+      <c r="B106" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B106" s="1" t="s">
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" s="1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
+      <c r="B107" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B107" s="1" t="s">
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
+      <c r="B108" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B108" s="1" t="s">
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" s="1" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
+      <c r="B109" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B109" s="1" t="s">
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="1" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
+      <c r="B110" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B110" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B112" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B112" s="1" t="s">
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="1" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
+      <c r="B113" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B113" s="1" t="s">
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" s="1" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
+      <c r="B114" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B114" s="1" t="s">
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="1" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
+      <c r="B115" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B115" s="1" t="s">
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" s="1" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
+      <c r="B116" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B116" s="1" t="s">
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" s="1" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
+      <c r="B117" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B117" s="1" t="s">
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="1" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
+      <c r="B118" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B118" s="1" t="s">
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="1" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
+      <c r="B119" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B119" s="1" t="s">
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="1" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
+      <c r="B120" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B120" s="1" t="s">
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" s="1" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
+      <c r="B121" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B121" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>14</v>
       </c>
@@ -2279,87 +2281,87 @@
         <v>14</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B123" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B123" s="1" t="s">
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="1" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="1" t="s">
+      <c r="B124" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B124" s="1" t="s">
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="1" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="1" t="s">
+      <c r="B125" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B125" s="1" t="s">
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="1" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="1" t="s">
+      <c r="B126" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B126" s="1" t="s">
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="1" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
+      <c r="B127" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="B127" s="1" t="s">
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="1" t="s">
+      <c r="B128" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B128" s="1" t="s">
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="1" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="1" t="s">
+      <c r="B129" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B129" s="1" t="s">
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="1" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="1" t="s">
+      <c r="B130" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="B130" s="1" t="s">
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="1" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="1" t="s">
+      <c r="B131" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B131" s="1" t="s">
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="1" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="1" t="s">
+      <c r="B132" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="B132" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>14</v>
       </c>
@@ -2367,79 +2369,79 @@
         <v>14</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B134" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="B134" s="1" t="s">
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" s="1" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="1" t="s">
+      <c r="B135" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="B135" s="1" t="s">
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" s="1" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="1" t="s">
+      <c r="B136" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="B136" s="1" t="s">
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" s="1" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="1" t="s">
+      <c r="B137" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="B137" s="1" t="s">
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" s="1" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="1" t="s">
+      <c r="B138" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="B138" s="1" t="s">
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" s="1" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="1" t="s">
+      <c r="B139" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="B139" s="1" t="s">
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" s="1" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="1" t="s">
+      <c r="B140" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B140" s="1" t="s">
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" s="1" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="1" t="s">
+      <c r="B141" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="B141" s="1" t="s">
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" s="1" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="1" t="s">
+      <c r="B142" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="B142" s="1" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>14</v>
       </c>
@@ -2447,55 +2449,55 @@
         <v>14</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B144" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="B144" s="1" t="s">
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" s="1" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" s="1" t="s">
+      <c r="B145" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="B145" s="1" t="s">
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" s="1" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="1" t="s">
+      <c r="B146" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="B146" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="1" t="s">
+      <c r="B147" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="B147" s="1" t="s">
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" s="1" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="1" t="s">
+      <c r="B148" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="B148" s="1" t="s">
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" s="1" t="s">
         <v>274</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="1" t="s">
-        <v>275</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>14</v>
       </c>
@@ -2503,39 +2505,39 @@
         <v>14</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B151" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="B151" s="1" t="s">
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" s="1" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="1" t="s">
+      <c r="B152" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="B152" s="1" t="s">
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" s="1" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="1" t="s">
+      <c r="B153" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B153" s="1" t="s">
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" s="1" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" s="1" t="s">
-        <v>282</v>
-      </c>
       <c r="B154" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>14</v>
       </c>
@@ -2543,28 +2545,28 @@
         <v>14</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B156" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="B156" s="1" t="s">
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" s="1" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="1" t="s">
+      <c r="B157" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B157" s="1" t="s">
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158" s="1" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="1" t="s">
+      <c r="B158" s="1" t="s">
         <v>287</v>
-      </c>
-      <c r="B158" s="1" t="s">
-        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -2581,7 +2583,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
v1.9 fixed categories, need to delete database and migrations and restart
</commit_message>
<xml_diff>
--- a/Categories.xlsx
+++ b/Categories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neerajsudhakar/BSA_Web_MVP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C274C9-206A-004A-8F20-B1B9B468F83B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF0D3D8-CAB4-7147-BEEC-C9382E701063}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{1FDBD104-F759-4528-9157-7D799DE775EC}"/>
   </bookViews>
@@ -911,7 +911,7 @@
     <t>Theoretical Economics</t>
   </si>
   <si>
-    <t>Pattern Formation and Solutons</t>
+    <t>Pattern Formation and Solutions</t>
   </si>
 </sst>
 </file>
@@ -1295,8 +1295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D48CA84-7451-4B0B-8098-0AC9374BDE6F}">
   <dimension ref="A1:B158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>